<commit_message>
edit code that checking nan input
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects.id\Abdul Asiz\auto-upload-produk-akulaku2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects.id\Abdul Asiz\auto-upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE0B586-2277-42A0-BE9D-96857B42C8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7853D4-1D5F-4E9E-B3FA-59CB53B1635B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="-11640" windowWidth="20730" windowHeight="11310" xr2:uid="{8DBE5AA8-0344-4128-9809-F26E693CDA50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{8DBE5AA8-0344-4128-9809-F26E693CDA50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4151" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4146" uniqueCount="553">
   <si>
     <t>Sub Kategori 1</t>
   </si>
@@ -2072,6 +2072,9 @@
   </si>
   <si>
     <t>ok100</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/eldy/image/upload/w_800,h_800/l_Bingkai_1,w_810,h_810/x9bidibxkz/1-1.jpg</t>
   </si>
 </sst>
 </file>
@@ -2773,7 +2776,7 @@
   <dimension ref="A1:AY11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3068,9 +3071,7 @@
       <c r="AL2" t="s">
         <v>531</v>
       </c>
-      <c r="AM2" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="AM2" s="3"/>
       <c r="AN2" s="3" t="s">
         <v>77</v>
       </c>
@@ -3134,9 +3135,7 @@
       <c r="AD3" t="s">
         <v>550</v>
       </c>
-      <c r="AM3" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="AM3" s="3"/>
       <c r="AN3" s="3" t="s">
         <v>77</v>
       </c>
@@ -3217,9 +3216,7 @@
       <c r="AF4" t="s">
         <v>538</v>
       </c>
-      <c r="AM4" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="AM4" s="3"/>
       <c r="AN4" s="3" t="s">
         <v>77</v>
       </c>
@@ -3264,9 +3261,6 @@
       <c r="D5" t="s">
         <v>532</v>
       </c>
-      <c r="E5" t="s">
-        <v>150</v>
-      </c>
       <c r="I5">
         <v>2000</v>
       </c>
@@ -3277,7 +3271,7 @@
         <v>543</v>
       </c>
       <c r="AM5" s="3" t="s">
-        <v>77</v>
+        <v>552</v>
       </c>
       <c r="AN5" s="3"/>
       <c r="AO5" s="3"/>
@@ -3337,9 +3331,7 @@
       <c r="AC6" t="s">
         <v>548</v>
       </c>
-      <c r="AM6" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="AM6" s="3"/>
       <c r="AN6" s="3" t="s">
         <v>77</v>
       </c>
@@ -3395,30 +3387,25 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="AM2" r:id="rId1" location=".jpg" xr:uid="{64805C30-D242-4AA5-93EA-CDF69DE3DA38}"/>
-    <hyperlink ref="AN2" r:id="rId2" location=".jpg" xr:uid="{106BCF7D-9918-4C3D-A914-E5F4F400E9D8}"/>
-    <hyperlink ref="AM3" r:id="rId3" location=".jpg" xr:uid="{A6E09CF9-5175-437A-89AA-9BF16EA0784F}"/>
-    <hyperlink ref="AM4" r:id="rId4" location=".jpg" xr:uid="{B554FE4E-6AA0-4A85-B1B1-37C18A792F5E}"/>
-    <hyperlink ref="AM5" r:id="rId5" location=".jpg" xr:uid="{B107155C-1A7C-49A6-B7EE-3E0779AB1FE1}"/>
-    <hyperlink ref="AM6" r:id="rId6" location=".jpg" xr:uid="{99F76BF1-3CB8-4CDA-B2C1-DE608A411C30}"/>
-    <hyperlink ref="AN3" r:id="rId7" location=".jpg" xr:uid="{3CB177A4-D66A-428C-8216-2120AF098F6C}"/>
-    <hyperlink ref="AN4" r:id="rId8" location=".jpg" xr:uid="{98009384-44BC-4658-A756-B750CD7B3FB6}"/>
-    <hyperlink ref="AN6" r:id="rId9" location=".jpg" xr:uid="{30E77631-CBD6-4533-94A8-90B788541E22}"/>
-    <hyperlink ref="AO3" r:id="rId10" location=".jpg" xr:uid="{D68404C0-CBEB-4C70-9A9F-89C1635C295E}"/>
-    <hyperlink ref="AP3" r:id="rId11" location=".jpg" xr:uid="{1A6A96A8-309B-4987-89A2-C8D881D54CAD}"/>
-    <hyperlink ref="AO4" r:id="rId12" location=".jpg" xr:uid="{246578D8-5C3F-4FDB-818D-1AF2FAB43987}"/>
-    <hyperlink ref="AQ4" r:id="rId13" location=".jpg" xr:uid="{F38C8D40-96D6-4817-88B9-0598DA04F77F}"/>
-    <hyperlink ref="AP4" r:id="rId14" location=".jpg" xr:uid="{11DD338D-A170-49BE-894D-89AE664EAAD0}"/>
-    <hyperlink ref="AR4" r:id="rId15" location=".jpg" xr:uid="{BC5114A2-CDD4-4713-A1DF-97AF9CA79CE5}"/>
-    <hyperlink ref="AO6" r:id="rId16" location=".jpg" xr:uid="{D0E54410-0312-4960-8243-E90B359CB6E4}"/>
-    <hyperlink ref="AP6" r:id="rId17" location=".jpg" xr:uid="{09711A93-F800-4E2D-AB56-EA9D20E1B8B3}"/>
-    <hyperlink ref="AQ6" r:id="rId18" location=".jpg" xr:uid="{72C081BD-757B-42A6-B536-A2AEB50C45EB}"/>
-    <hyperlink ref="AR6" r:id="rId19" location=".jpg" xr:uid="{5F2587AB-154D-47C1-991B-9915B290FBCE}"/>
-    <hyperlink ref="AS6" r:id="rId20" location=".jpg" xr:uid="{77F23BA5-FB33-43D0-93ED-41961E329E9C}"/>
-    <hyperlink ref="AT6" r:id="rId21" location=".jpg" xr:uid="{2A1840E4-1619-48CB-A75E-B1F7DCB034F4}"/>
+    <hyperlink ref="AN2" r:id="rId1" location=".jpg" xr:uid="{106BCF7D-9918-4C3D-A914-E5F4F400E9D8}"/>
+    <hyperlink ref="AN3" r:id="rId2" location=".jpg" xr:uid="{3CB177A4-D66A-428C-8216-2120AF098F6C}"/>
+    <hyperlink ref="AN4" r:id="rId3" location=".jpg" xr:uid="{98009384-44BC-4658-A756-B750CD7B3FB6}"/>
+    <hyperlink ref="AN6" r:id="rId4" location=".jpg" xr:uid="{30E77631-CBD6-4533-94A8-90B788541E22}"/>
+    <hyperlink ref="AO3" r:id="rId5" location=".jpg" xr:uid="{D68404C0-CBEB-4C70-9A9F-89C1635C295E}"/>
+    <hyperlink ref="AP3" r:id="rId6" location=".jpg" xr:uid="{1A6A96A8-309B-4987-89A2-C8D881D54CAD}"/>
+    <hyperlink ref="AO4" r:id="rId7" location=".jpg" xr:uid="{246578D8-5C3F-4FDB-818D-1AF2FAB43987}"/>
+    <hyperlink ref="AQ4" r:id="rId8" location=".jpg" xr:uid="{F38C8D40-96D6-4817-88B9-0598DA04F77F}"/>
+    <hyperlink ref="AP4" r:id="rId9" location=".jpg" xr:uid="{11DD338D-A170-49BE-894D-89AE664EAAD0}"/>
+    <hyperlink ref="AR4" r:id="rId10" location=".jpg" xr:uid="{BC5114A2-CDD4-4713-A1DF-97AF9CA79CE5}"/>
+    <hyperlink ref="AO6" r:id="rId11" location=".jpg" xr:uid="{D0E54410-0312-4960-8243-E90B359CB6E4}"/>
+    <hyperlink ref="AP6" r:id="rId12" location=".jpg" xr:uid="{09711A93-F800-4E2D-AB56-EA9D20E1B8B3}"/>
+    <hyperlink ref="AQ6" r:id="rId13" location=".jpg" xr:uid="{72C081BD-757B-42A6-B536-A2AEB50C45EB}"/>
+    <hyperlink ref="AR6" r:id="rId14" location=".jpg" xr:uid="{5F2587AB-154D-47C1-991B-9915B290FBCE}"/>
+    <hyperlink ref="AS6" r:id="rId15" location=".jpg" xr:uid="{77F23BA5-FB33-43D0-93ED-41961E329E9C}"/>
+    <hyperlink ref="AT6" r:id="rId16" location=".jpg" xr:uid="{2A1840E4-1619-48CB-A75E-B1F7DCB034F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId22"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>